<commit_message>
show system info to display functions added with related variables
</commit_message>
<xml_diff>
--- a/project pins.xlsx
+++ b/project pins.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Board ports" sheetId="1" r:id="rId1"/>
@@ -441,7 +441,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="64">
   <si>
     <t>MCU</t>
   </si>
@@ -609,6 +609,30 @@
   </si>
   <si>
     <t>p0.24</t>
+  </si>
+  <si>
+    <t>÷</t>
+  </si>
+  <si>
+    <t>BS</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>Caller number</t>
   </si>
 </sst>
 </file>
@@ -693,7 +717,7 @@
       <name val="Tahoma"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -712,6 +736,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -875,7 +923,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -917,6 +965,42 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1224,7 +1308,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="F1:AG38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D17" zoomScale="82" zoomScaleNormal="82" workbookViewId="0">
+    <sheetView topLeftCell="A17" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
       <selection activeCell="U18" sqref="U18"/>
     </sheetView>
   </sheetViews>
@@ -1621,119 +1705,179 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:Q3"/>
+  <dimension ref="B2:Q10"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" customWidth="1"/>
-    <col min="2" max="17" width="4.140625" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" style="27" customWidth="1"/>
+    <col min="2" max="17" width="4.140625" style="27" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="27"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="1">
+      <c r="B2" s="28">
         <v>80</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="25">
         <v>81</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" s="25">
         <v>82</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="25">
         <v>83</v>
       </c>
-      <c r="F2" s="1">
+      <c r="F2" s="25">
         <v>84</v>
       </c>
-      <c r="G2" s="1">
+      <c r="G2" s="26">
         <v>85</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2" s="26">
         <v>86</v>
       </c>
-      <c r="I2" s="1">
+      <c r="I2" s="26">
         <v>87</v>
       </c>
-      <c r="J2" s="1">
+      <c r="J2" s="26">
         <v>88</v>
       </c>
-      <c r="K2" s="1">
+      <c r="K2" s="26">
         <v>89</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="O2" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="P2" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="Q2" s="26" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="3" spans="2:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="33" t="s">
         <v>36</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="K3" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L3" s="25" t="s">
         <v>47</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="M3" s="32" t="s">
         <v>48</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="N3" s="32" t="s">
         <v>49</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="O3" s="32" t="s">
         <v>50</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="P3" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="Q3" s="1" t="s">
+      <c r="Q3" s="32" t="s">
         <v>52</v>
       </c>
     </row>
+    <row r="6" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="C6" s="25"/>
+      <c r="D6" s="25"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="25"/>
+      <c r="G6" s="22" t="s">
+        <v>63</v>
+      </c>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="24"/>
+    </row>
+    <row r="7" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="25"/>
+      <c r="C7" s="25"/>
+      <c r="D7" s="25"/>
+      <c r="E7" s="25"/>
+      <c r="F7" s="25"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="33" t="s">
+        <v>59</v>
+      </c>
+      <c r="I7" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="J7" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="K7" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="L7" s="25"/>
+      <c r="M7" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="N7" s="30"/>
+      <c r="O7" s="30"/>
+      <c r="P7" s="30"/>
+      <c r="Q7" s="31"/>
+    </row>
+    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C10" s="27" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="G6:Q6"/>
+    <mergeCell ref="M7:Q7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
relays can controll by user in browser
</commit_message>
<xml_diff>
--- a/project pins.xlsx
+++ b/project pins.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Board ports" sheetId="1" r:id="rId1"/>
@@ -332,10 +332,17 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>قطع و وصل کننده خط 
-اتصال به سیم نارنجی رنگی که از رله خارج شده</t>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+وصل کردن خط تماس</t>
         </r>
       </text>
     </comment>
@@ -441,7 +448,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="87">
   <si>
     <t>MCU</t>
   </si>
@@ -506,9 +513,6 @@
     <t>p0.20</t>
   </si>
   <si>
-    <t>ethrnet</t>
-  </si>
-  <si>
     <t>p1.4</t>
   </si>
   <si>
@@ -602,9 +606,6 @@
     <t>CF</t>
   </si>
   <si>
-    <t>Uart - caller id</t>
-  </si>
-  <si>
     <t>p0.3</t>
   </si>
   <si>
@@ -633,6 +634,81 @@
   </si>
   <si>
     <t>Caller number</t>
+  </si>
+  <si>
+    <t>UART0 RX</t>
+  </si>
+  <si>
+    <t>Caller id interupt to read serial data</t>
+  </si>
+  <si>
+    <t>Ring detector pin</t>
+  </si>
+  <si>
+    <t>Tone detector interupt for read latched pins</t>
+  </si>
+  <si>
+    <t>Q1 LSB tone detector pin</t>
+  </si>
+  <si>
+    <t>Q2 tone detector pin</t>
+  </si>
+  <si>
+    <t>Q3  tone detector pin</t>
+  </si>
+  <si>
+    <t>Q4 MSB  tone detector pin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ethernet </t>
+  </si>
+  <si>
+    <t>LCD DB4</t>
+  </si>
+  <si>
+    <t>LCD DB5</t>
+  </si>
+  <si>
+    <t>LCD DB6</t>
+  </si>
+  <si>
+    <t>LCD DB7</t>
+  </si>
+  <si>
+    <t>LCD E</t>
+  </si>
+  <si>
+    <t>LCD RS</t>
+  </si>
+  <si>
+    <t>LCD RW</t>
+  </si>
+  <si>
+    <t>p0.5</t>
+  </si>
+  <si>
+    <t>p0.6</t>
+  </si>
+  <si>
+    <t>p0.7</t>
+  </si>
+  <si>
+    <t>p0.8</t>
+  </si>
+  <si>
+    <t>Relay 1</t>
+  </si>
+  <si>
+    <t>Relay 2</t>
+  </si>
+  <si>
+    <t>Relay 3</t>
+  </si>
+  <si>
+    <t>Relay 4</t>
+  </si>
+  <si>
+    <t>accept the call</t>
   </si>
 </sst>
 </file>
@@ -717,7 +793,7 @@
       <name val="Tahoma"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -760,6 +836,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="13">
     <border>
@@ -923,7 +1017,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -954,6 +1048,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -975,32 +1087,41 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1308,8 +1429,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="F1:AG38"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="U18" sqref="U18"/>
+    <sheetView topLeftCell="F18" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1324,7 +1445,7 @@
     <row r="4" spans="6:33" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="6:33" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F5" s="17" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -1389,11 +1510,11 @@
       <c r="AD6" s="1"/>
     </row>
     <row r="7" spans="6:33" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F7" s="19" t="s">
+      <c r="F7" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
+      <c r="G7" s="25"/>
+      <c r="H7" s="25"/>
     </row>
     <row r="8" spans="6:33" ht="32.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="6:33" ht="32.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1406,92 +1527,92 @@
       <c r="AF12" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="AG12" s="20" t="s">
+      <c r="AG12" s="26" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="6:33" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AE13" s="13"/>
       <c r="AF13" s="13"/>
-      <c r="AG13" s="21"/>
+      <c r="AG13" s="27"/>
     </row>
     <row r="14" spans="6:33" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AE14" s="1"/>
       <c r="AF14" s="1"/>
-      <c r="AG14" s="21"/>
+      <c r="AG14" s="27"/>
     </row>
     <row r="15" spans="6:33" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O15" s="18" t="s">
+      <c r="O15" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="P15" s="18"/>
-      <c r="Q15" s="18"/>
-      <c r="R15" s="18"/>
-      <c r="S15" s="18"/>
+      <c r="P15" s="24"/>
+      <c r="Q15" s="24"/>
+      <c r="R15" s="24"/>
+      <c r="S15" s="24"/>
       <c r="AE15" s="1"/>
       <c r="AF15" s="1"/>
-      <c r="AG15" s="21"/>
+      <c r="AG15" s="27"/>
     </row>
     <row r="16" spans="6:33" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O16" s="18"/>
-      <c r="P16" s="18"/>
-      <c r="Q16" s="18"/>
-      <c r="R16" s="18"/>
-      <c r="S16" s="18"/>
+      <c r="O16" s="24"/>
+      <c r="P16" s="24"/>
+      <c r="Q16" s="24"/>
+      <c r="R16" s="24"/>
+      <c r="S16" s="24"/>
       <c r="AE16" s="1"/>
       <c r="AF16" s="1"/>
     </row>
     <row r="17" spans="6:32" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O17" s="18"/>
-      <c r="P17" s="18"/>
-      <c r="Q17" s="18"/>
-      <c r="R17" s="18"/>
-      <c r="S17" s="18"/>
+      <c r="O17" s="24"/>
+      <c r="P17" s="24"/>
+      <c r="Q17" s="24"/>
+      <c r="R17" s="24"/>
+      <c r="S17" s="24"/>
       <c r="AE17" s="1"/>
       <c r="AF17" s="1"/>
     </row>
     <row r="18" spans="6:32" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O18" s="18"/>
-      <c r="P18" s="18"/>
-      <c r="Q18" s="18"/>
-      <c r="R18" s="18"/>
-      <c r="S18" s="18"/>
+      <c r="O18" s="24"/>
+      <c r="P18" s="24"/>
+      <c r="Q18" s="24"/>
+      <c r="R18" s="24"/>
+      <c r="S18" s="24"/>
       <c r="AE18" s="1"/>
       <c r="AF18" s="1"/>
     </row>
     <row r="19" spans="6:32" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O19" s="18"/>
-      <c r="P19" s="18"/>
-      <c r="Q19" s="18"/>
-      <c r="R19" s="18"/>
-      <c r="S19" s="18"/>
+      <c r="O19" s="24"/>
+      <c r="P19" s="24"/>
+      <c r="Q19" s="24"/>
+      <c r="R19" s="24"/>
+      <c r="S19" s="24"/>
       <c r="AE19" s="1"/>
       <c r="AF19" s="1"/>
     </row>
     <row r="20" spans="6:32" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O20" s="18"/>
-      <c r="P20" s="18"/>
-      <c r="Q20" s="18"/>
-      <c r="R20" s="18"/>
-      <c r="S20" s="18"/>
+      <c r="O20" s="24"/>
+      <c r="P20" s="24"/>
+      <c r="Q20" s="24"/>
+      <c r="R20" s="24"/>
+      <c r="S20" s="24"/>
       <c r="AE20" s="1"/>
       <c r="AF20" s="1"/>
     </row>
     <row r="21" spans="6:32" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O21" s="18"/>
-      <c r="P21" s="18"/>
-      <c r="Q21" s="18"/>
-      <c r="R21" s="18"/>
-      <c r="S21" s="18"/>
+      <c r="O21" s="24"/>
+      <c r="P21" s="24"/>
+      <c r="Q21" s="24"/>
+      <c r="R21" s="24"/>
+      <c r="S21" s="24"/>
       <c r="AE21" s="1"/>
       <c r="AF21" s="1"/>
     </row>
     <row r="22" spans="6:32" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O22" s="18"/>
-      <c r="P22" s="18"/>
-      <c r="Q22" s="18"/>
-      <c r="R22" s="18"/>
-      <c r="S22" s="18"/>
+      <c r="O22" s="24"/>
+      <c r="P22" s="24"/>
+      <c r="Q22" s="24"/>
+      <c r="R22" s="24"/>
+      <c r="S22" s="24"/>
       <c r="AE22" s="1"/>
       <c r="AF22" s="1"/>
     </row>
@@ -1532,7 +1653,7 @@
         <v>6</v>
       </c>
       <c r="I31" s="12" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
@@ -1600,11 +1721,11 @@
       <c r="AD32" s="1"/>
     </row>
     <row r="33" spans="6:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F33" s="19" t="s">
+      <c r="F33" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
+      <c r="G33" s="25"/>
+      <c r="H33" s="25"/>
     </row>
     <row r="34" spans="6:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" spans="6:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1626,79 +1747,283 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:D11"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="3" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="36" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
+    <col min="5" max="5" width="41.140625" style="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="20"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="35"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="20"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="35"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="20"/>
+      <c r="B3" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="E3" s="35" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="20"/>
+      <c r="B4" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="D2" t="s">
+      <c r="C4" s="34"/>
+      <c r="D4" s="41" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="42" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="20"/>
+      <c r="B5" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="34"/>
+      <c r="D5" s="41" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="42" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="20"/>
+      <c r="B6" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="34"/>
+      <c r="D6" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="42" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="20"/>
+      <c r="B7" s="20" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="34"/>
+      <c r="D7" s="41" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="42" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="20"/>
+      <c r="B8" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="34"/>
+      <c r="D8" s="41" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="42" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="20"/>
+      <c r="B9" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="34"/>
+      <c r="D9" s="20" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="E9" s="35" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="20"/>
+      <c r="B10" s="20" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="C10" s="34"/>
+      <c r="D10" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="35" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="20"/>
+      <c r="B11" s="20" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>30</v>
-      </c>
+      <c r="C11" s="34"/>
+      <c r="D11" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="35" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="20"/>
+      <c r="B12" s="37" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="38" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="E12" s="40" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="20"/>
+      <c r="B13" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="38" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="E13" s="40" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="20"/>
+      <c r="B14" s="37" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="38" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" s="39" t="s">
+        <v>80</v>
+      </c>
+      <c r="E14" s="40" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="20"/>
+      <c r="B15" s="37" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="38" t="s">
+        <v>74</v>
+      </c>
+      <c r="D15" s="39" t="s">
+        <v>81</v>
+      </c>
+      <c r="E15" s="40" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="20"/>
+      <c r="B16" s="37" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="20"/>
+      <c r="E16" s="35"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="20"/>
+      <c r="B17" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="D17" s="20"/>
+      <c r="E17" s="35"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="20"/>
+      <c r="B18" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="38" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" s="20"/>
+      <c r="E18" s="35"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="35"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="20"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="35"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="20"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="35"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="35"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="20"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="35"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="35"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="20"/>
+      <c r="B23" s="20"/>
+      <c r="C23" s="35"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="35"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C3:C11"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1707,170 +2032,170 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:Q10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B7" sqref="B7:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" style="27" customWidth="1"/>
-    <col min="2" max="17" width="4.140625" style="27" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="27"/>
+    <col min="1" max="1" width="4.85546875" style="20" customWidth="1"/>
+    <col min="2" max="17" width="4.140625" style="20" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="20"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="28">
+      <c r="B2" s="21">
         <v>80</v>
       </c>
-      <c r="C2" s="25">
+      <c r="C2" s="18">
         <v>81</v>
       </c>
-      <c r="D2" s="25">
+      <c r="D2" s="18">
         <v>82</v>
       </c>
-      <c r="E2" s="25">
+      <c r="E2" s="18">
         <v>83</v>
       </c>
-      <c r="F2" s="25">
+      <c r="F2" s="18">
         <v>84</v>
       </c>
-      <c r="G2" s="26">
+      <c r="G2" s="19">
         <v>85</v>
       </c>
-      <c r="H2" s="26">
+      <c r="H2" s="19">
         <v>86</v>
       </c>
-      <c r="I2" s="26">
+      <c r="I2" s="19">
         <v>87</v>
       </c>
-      <c r="J2" s="26">
+      <c r="J2" s="19">
         <v>88</v>
       </c>
-      <c r="K2" s="26">
+      <c r="K2" s="19">
         <v>89</v>
       </c>
-      <c r="L2" s="26" t="s">
+      <c r="L2" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="M2" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="M2" s="26" t="s">
+      <c r="N2" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="N2" s="26" t="s">
+      <c r="O2" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="O2" s="26" t="s">
+      <c r="P2" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="P2" s="26" t="s">
+      <c r="Q2" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="Q2" s="26" t="s">
+    </row>
+    <row r="3" spans="2:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3" s="23" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" s="18" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="3" spans="2:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="25" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="D3" s="25" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="F3" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="G3" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="H3" s="33" t="s">
-        <v>36</v>
-      </c>
-      <c r="I3" s="33" t="s">
-        <v>37</v>
-      </c>
-      <c r="J3" s="33" t="s">
-        <v>38</v>
-      </c>
-      <c r="K3" s="33" t="s">
-        <v>39</v>
-      </c>
-      <c r="L3" s="25" t="s">
+      <c r="M3" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="M3" s="32" t="s">
+      <c r="N3" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="N3" s="32" t="s">
+      <c r="O3" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="O3" s="32" t="s">
+      <c r="P3" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="P3" s="32" t="s">
+      <c r="Q3" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="Q3" s="32" t="s">
-        <v>52</v>
-      </c>
     </row>
     <row r="6" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6" s="29"/>
+      <c r="I6" s="29"/>
+      <c r="J6" s="29"/>
+      <c r="K6" s="29"/>
+      <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
+      <c r="N6" s="29"/>
+      <c r="O6" s="29"/>
+      <c r="P6" s="29"/>
+      <c r="Q6" s="30"/>
+    </row>
+    <row r="7" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="18"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="22" t="s">
-        <v>63</v>
-      </c>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="23"/>
-      <c r="Q6" s="24"/>
-    </row>
-    <row r="7" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="25"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="G7" s="25"/>
-      <c r="H7" s="33" t="s">
+      <c r="I7" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="J7" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="I7" s="33" t="s">
+      <c r="K7" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="J7" s="33" t="s">
-        <v>61</v>
-      </c>
-      <c r="K7" s="33" t="s">
-        <v>62</v>
-      </c>
-      <c r="L7" s="25"/>
-      <c r="M7" s="29" t="s">
-        <v>58</v>
-      </c>
-      <c r="N7" s="30"/>
-      <c r="O7" s="30"/>
-      <c r="P7" s="30"/>
-      <c r="Q7" s="31"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="31" t="s">
+        <v>56</v>
+      </c>
+      <c r="N7" s="32"/>
+      <c r="O7" s="32"/>
+      <c r="P7" s="32"/>
+      <c r="Q7" s="33"/>
     </row>
     <row r="10" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="C10" s="27" t="s">
-        <v>56</v>
+      <c r="C10" s="20" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new algorithm for validation tone code
</commit_message>
<xml_diff>
--- a/project pins.xlsx
+++ b/project pins.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Board ports" sheetId="1" r:id="rId1"/>
     <sheet name="Pins" sheetId="2" r:id="rId2"/>
-    <sheet name="LCD" sheetId="3" r:id="rId3"/>
+    <sheet name="EEPROM" sheetId="4" r:id="rId3"/>
+    <sheet name="LCD" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -44,6 +45,54 @@
         </r>
       </text>
     </comment>
+    <comment ref="P5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Relay 2</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Relay 4</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="Y5" authorId="0" shapeId="0">
       <text>
         <r>
@@ -114,6 +163,54 @@
           </rPr>
           <t xml:space="preserve">
 Q4</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Relay 1</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="Q6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Relay 3</t>
         </r>
       </text>
     </comment>
@@ -448,7 +545,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="102">
   <si>
     <t>MCU</t>
   </si>
@@ -612,9 +709,6 @@
     <t>p0.24</t>
   </si>
   <si>
-    <t>÷</t>
-  </si>
-  <si>
     <t>BS</t>
   </si>
   <si>
@@ -709,6 +803,54 @@
   </si>
   <si>
     <t>accept the call</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>I/O</t>
+  </si>
+  <si>
+    <t>relay 1</t>
+  </si>
+  <si>
+    <t>relay 2</t>
+  </si>
+  <si>
+    <t>relay 3</t>
+  </si>
+  <si>
+    <t>relay 4</t>
+  </si>
+  <si>
+    <t>number 1</t>
+  </si>
+  <si>
+    <t>number 2</t>
+  </si>
+  <si>
+    <t>number 3</t>
+  </si>
+  <si>
+    <t>number 4</t>
+  </si>
+  <si>
+    <t>number 5</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>`</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>#</t>
   </si>
 </sst>
 </file>
@@ -759,13 +901,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="22"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="20"/>
       <color theme="1"/>
@@ -792,8 +927,15 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
     </font>
+    <font>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -854,8 +996,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -1013,39 +1167,147 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1064,6 +1326,85 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1078,6 +1419,63 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="180"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1096,32 +1494,14 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1429,9 +1809,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="F1:AG38"/>
   <sheetViews>
-    <sheetView topLeftCell="F18" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="30" zoomScaleNormal="30" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1444,34 +1822,38 @@
     <row r="3" spans="6:33" ht="32.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="6:33" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="6:33" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F5" s="17" t="s">
+      <c r="F5" s="27" t="s">
         <v>52</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="16"/>
-      <c r="L5" s="16"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
       <c r="M5" s="1"/>
       <c r="N5" s="2"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q5" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="R5" s="2"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
       <c r="W5" s="1"/>
-      <c r="X5" s="6"/>
-      <c r="Y5" s="17" t="s">
+      <c r="X5" s="5"/>
+      <c r="Y5" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="Z5" s="17" t="s">
+      <c r="Z5" s="27" t="s">
         <v>19</v>
       </c>
-      <c r="AA5" s="17" t="s">
+      <c r="AA5" s="27" t="s">
         <v>8</v>
       </c>
       <c r="AB5" s="2"/>
@@ -1483,26 +1865,30 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="16"/>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
-      <c r="Q6" s="1"/>
-      <c r="R6" s="1"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q6" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="R6" s="2"/>
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
       <c r="V6" s="1"/>
       <c r="W6" s="1"/>
       <c r="X6" s="1"/>
-      <c r="Y6" s="9"/>
-      <c r="Z6" s="17" t="s">
+      <c r="Y6" s="8"/>
+      <c r="Z6" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="AA6" s="17" t="s">
+      <c r="AA6" s="27" t="s">
         <v>20</v>
       </c>
       <c r="AB6" s="2"/>
@@ -1510,109 +1896,109 @@
       <c r="AD6" s="1"/>
     </row>
     <row r="7" spans="6:33" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F7" s="25" t="s">
+      <c r="F7" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="25"/>
-      <c r="H7" s="25"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
     </row>
     <row r="8" spans="6:33" ht="32.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="9" spans="6:33" ht="32.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="6:33" ht="32.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="6:33" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="6:33" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="AE12" s="12" t="s">
+      <c r="AE12" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="AF12" s="12" t="s">
+      <c r="AF12" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="AG12" s="26" t="s">
+      <c r="AG12" s="48" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="6:33" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="AE13" s="13"/>
-      <c r="AF13" s="13"/>
-      <c r="AG13" s="27"/>
+      <c r="AE13" s="10"/>
+      <c r="AF13" s="10"/>
+      <c r="AG13" s="49"/>
     </row>
     <row r="14" spans="6:33" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="AE14" s="1"/>
       <c r="AF14" s="1"/>
-      <c r="AG14" s="27"/>
+      <c r="AG14" s="49"/>
     </row>
     <row r="15" spans="6:33" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O15" s="24" t="s">
+      <c r="O15" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="P15" s="24"/>
-      <c r="Q15" s="24"/>
-      <c r="R15" s="24"/>
-      <c r="S15" s="24"/>
+      <c r="P15" s="46"/>
+      <c r="Q15" s="46"/>
+      <c r="R15" s="46"/>
+      <c r="S15" s="46"/>
       <c r="AE15" s="1"/>
       <c r="AF15" s="1"/>
-      <c r="AG15" s="27"/>
+      <c r="AG15" s="49"/>
     </row>
     <row r="16" spans="6:33" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O16" s="24"/>
-      <c r="P16" s="24"/>
-      <c r="Q16" s="24"/>
-      <c r="R16" s="24"/>
-      <c r="S16" s="24"/>
+      <c r="O16" s="46"/>
+      <c r="P16" s="46"/>
+      <c r="Q16" s="46"/>
+      <c r="R16" s="46"/>
+      <c r="S16" s="46"/>
       <c r="AE16" s="1"/>
       <c r="AF16" s="1"/>
     </row>
     <row r="17" spans="6:32" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O17" s="24"/>
-      <c r="P17" s="24"/>
-      <c r="Q17" s="24"/>
-      <c r="R17" s="24"/>
-      <c r="S17" s="24"/>
+      <c r="O17" s="46"/>
+      <c r="P17" s="46"/>
+      <c r="Q17" s="46"/>
+      <c r="R17" s="46"/>
+      <c r="S17" s="46"/>
       <c r="AE17" s="1"/>
       <c r="AF17" s="1"/>
     </row>
     <row r="18" spans="6:32" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O18" s="24"/>
-      <c r="P18" s="24"/>
-      <c r="Q18" s="24"/>
-      <c r="R18" s="24"/>
-      <c r="S18" s="24"/>
+      <c r="O18" s="46"/>
+      <c r="P18" s="46"/>
+      <c r="Q18" s="46"/>
+      <c r="R18" s="46"/>
+      <c r="S18" s="46"/>
       <c r="AE18" s="1"/>
       <c r="AF18" s="1"/>
     </row>
     <row r="19" spans="6:32" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O19" s="24"/>
-      <c r="P19" s="24"/>
-      <c r="Q19" s="24"/>
-      <c r="R19" s="24"/>
-      <c r="S19" s="24"/>
+      <c r="O19" s="46"/>
+      <c r="P19" s="46"/>
+      <c r="Q19" s="46"/>
+      <c r="R19" s="46"/>
+      <c r="S19" s="46"/>
       <c r="AE19" s="1"/>
       <c r="AF19" s="1"/>
     </row>
     <row r="20" spans="6:32" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O20" s="24"/>
-      <c r="P20" s="24"/>
-      <c r="Q20" s="24"/>
-      <c r="R20" s="24"/>
-      <c r="S20" s="24"/>
+      <c r="O20" s="46"/>
+      <c r="P20" s="46"/>
+      <c r="Q20" s="46"/>
+      <c r="R20" s="46"/>
+      <c r="S20" s="46"/>
       <c r="AE20" s="1"/>
       <c r="AF20" s="1"/>
     </row>
     <row r="21" spans="6:32" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O21" s="24"/>
-      <c r="P21" s="24"/>
-      <c r="Q21" s="24"/>
-      <c r="R21" s="24"/>
-      <c r="S21" s="24"/>
+      <c r="O21" s="46"/>
+      <c r="P21" s="46"/>
+      <c r="Q21" s="46"/>
+      <c r="R21" s="46"/>
+      <c r="S21" s="46"/>
       <c r="AE21" s="1"/>
       <c r="AF21" s="1"/>
     </row>
     <row r="22" spans="6:32" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O22" s="24"/>
-      <c r="P22" s="24"/>
-      <c r="Q22" s="24"/>
-      <c r="R22" s="24"/>
-      <c r="S22" s="24"/>
+      <c r="O22" s="46"/>
+      <c r="P22" s="46"/>
+      <c r="Q22" s="46"/>
+      <c r="R22" s="46"/>
+      <c r="S22" s="46"/>
       <c r="AE22" s="1"/>
       <c r="AF22" s="1"/>
     </row>
@@ -1636,23 +2022,23 @@
       <c r="AE27" s="3"/>
       <c r="AF27" s="3"/>
     </row>
-    <row r="28" spans="6:32" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="AE28" s="5" t="s">
+    <row r="28" spans="6:32" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AE28" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="AF28" s="5" t="s">
+      <c r="AF28" s="27" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="29" spans="6:32" ht="32.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="6:32" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="31" spans="6:32" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F31" s="7"/>
-      <c r="G31" s="6"/>
-      <c r="H31" s="12" t="s">
+      <c r="F31" s="6"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="I31" s="12" t="s">
+      <c r="I31" s="27" t="s">
         <v>53</v>
       </c>
       <c r="J31" s="1"/>
@@ -1667,14 +2053,14 @@
       <c r="S31" s="1"/>
       <c r="T31" s="1"/>
       <c r="U31" s="1"/>
-      <c r="V31" s="6"/>
-      <c r="W31" s="11" t="s">
+      <c r="V31" s="5"/>
+      <c r="W31" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="X31" s="11" t="s">
+      <c r="X31" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="Y31" s="11" t="s">
+      <c r="Y31" s="27" t="s">
         <v>15</v>
       </c>
       <c r="Z31" s="2"/>
@@ -1684,10 +2070,10 @@
       <c r="AD31" s="1"/>
     </row>
     <row r="32" spans="6:32" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F32" s="8"/>
+      <c r="F32" s="7"/>
       <c r="G32" s="1"/>
-      <c r="H32" s="9"/>
-      <c r="I32" s="12" t="s">
+      <c r="H32" s="8"/>
+      <c r="I32" s="27" t="s">
         <v>7</v>
       </c>
       <c r="J32" s="2"/>
@@ -1702,18 +2088,18 @@
       <c r="S32" s="1"/>
       <c r="T32" s="1"/>
       <c r="U32" s="1"/>
-      <c r="V32" s="6"/>
-      <c r="W32" s="11" t="s">
+      <c r="V32" s="5"/>
+      <c r="W32" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="X32" s="15" t="s">
+      <c r="X32" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="Y32" s="11" t="s">
+      <c r="Y32" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="Z32" s="10"/>
-      <c r="AA32" s="11" t="s">
+      <c r="Z32" s="9"/>
+      <c r="AA32" s="27" t="s">
         <v>16</v>
       </c>
       <c r="AB32" s="2"/>
@@ -1721,11 +2107,11 @@
       <c r="AD32" s="1"/>
     </row>
     <row r="33" spans="6:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F33" s="25" t="s">
+      <c r="F33" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="G33" s="25"/>
-      <c r="H33" s="25"/>
+      <c r="G33" s="47"/>
+      <c r="H33" s="47"/>
     </row>
     <row r="34" spans="6:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" spans="6:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1747,282 +2133,338 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="36" customWidth="1"/>
-    <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="41.140625" style="36" customWidth="1"/>
+    <col min="2" max="2" width="41.85546875" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" style="34" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10" style="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="20"/>
-      <c r="B1" s="20"/>
-      <c r="C1" s="35"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="35"/>
+      <c r="A1" s="15"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" s="15"/>
+      <c r="E1" s="19"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="20"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="35"/>
+      <c r="A2" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="50" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" s="15"/>
+      <c r="E2" s="19"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
-      <c r="B3" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="34" t="s">
+      <c r="A3" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="50"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="50"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="50"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="50"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="50"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="50"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="50"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="50"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="D3" s="20" t="s">
+      <c r="C11" s="34" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>72</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="C16" s="34" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="21" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="C17" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="D17" s="15"/>
+      <c r="E17" s="19"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="20"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="19"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="15"/>
+      <c r="B19" s="19"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="19"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="15"/>
+      <c r="B20" s="19"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="19"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="E3" s="35" t="s">
+      <c r="B21" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21" s="15"/>
+      <c r="E21" s="19"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="C22" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="D22" s="15"/>
+      <c r="E22" s="19"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="23" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="D23" s="15"/>
+      <c r="E23" s="19"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="23" t="s">
+        <v>79</v>
+      </c>
+      <c r="B24" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" s="34" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="23" t="s">
+        <v>80</v>
+      </c>
+      <c r="B25" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" s="34" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="20"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" s="34" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B28" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="34" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" s="34" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="C30" s="34" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="C31" s="34" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" s="33" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="20"/>
-      <c r="B4" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="34"/>
-      <c r="D4" s="41" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" s="42" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="20"/>
-      <c r="B5" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="34"/>
-      <c r="D5" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="42" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
-      <c r="B6" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="34"/>
-      <c r="D6" s="41" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" s="42" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="20"/>
-      <c r="B7" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="34"/>
-      <c r="D7" s="41" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="42" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="20"/>
-      <c r="B8" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="34"/>
-      <c r="D8" s="41" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" s="42" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="20"/>
-      <c r="B9" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="34"/>
-      <c r="D9" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="E9" s="35" t="s">
+      <c r="C32" s="34" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="33" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="20"/>
-      <c r="B10" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="34"/>
-      <c r="D10" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="E10" s="35" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="20"/>
-      <c r="B11" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="20" t="s">
+      <c r="C33" s="34" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="35" t="s">
+      <c r="B34" s="33" t="s">
+        <v>85</v>
+      </c>
+      <c r="C34" s="34" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="20"/>
-      <c r="B12" s="37" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="38" t="s">
-        <v>71</v>
-      </c>
-      <c r="D12" s="39" t="s">
-        <v>78</v>
-      </c>
-      <c r="E12" s="40" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="20"/>
-      <c r="B13" s="37" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="38" t="s">
-        <v>72</v>
-      </c>
-      <c r="D13" s="39" t="s">
-        <v>79</v>
-      </c>
-      <c r="E13" s="40" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="20"/>
-      <c r="B14" s="37" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="D14" s="39" t="s">
-        <v>80</v>
-      </c>
-      <c r="E14" s="40" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="20"/>
-      <c r="B15" s="37" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="38" t="s">
-        <v>74</v>
-      </c>
-      <c r="D15" s="39" t="s">
-        <v>81</v>
-      </c>
-      <c r="E15" s="40" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="20"/>
-      <c r="B16" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="38" t="s">
-        <v>75</v>
-      </c>
-      <c r="D16" s="20"/>
-      <c r="E16" s="35"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="20"/>
-      <c r="B17" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="D17" s="20"/>
-      <c r="E17" s="35"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
-      <c r="B18" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="38" t="s">
-        <v>77</v>
-      </c>
-      <c r="D18" s="20"/>
-      <c r="E18" s="35"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="35"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="20"/>
-      <c r="B20" s="20"/>
-      <c r="C20" s="35"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="35"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="20"/>
-      <c r="B21" s="20"/>
-      <c r="C21" s="35"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="35"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="20"/>
-      <c r="B22" s="20"/>
-      <c r="C22" s="35"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="35"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="20"/>
-      <c r="B23" s="20"/>
-      <c r="C23" s="35"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C3:C11"/>
+    <mergeCell ref="B2:B10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2030,173 +2472,734 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:Q10"/>
+  <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:F7"/>
+    <sheetView topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" style="20" customWidth="1"/>
-    <col min="2" max="17" width="4.140625" style="20" customWidth="1"/>
-    <col min="18" max="16384" width="9.140625" style="20"/>
+    <col min="1" max="1" width="9.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="35"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="43">
+        <v>1</v>
+      </c>
+      <c r="B2" s="57" t="s">
+        <v>89</v>
+      </c>
+      <c r="C2" s="75" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="44">
+        <v>2</v>
+      </c>
+      <c r="B3" s="58"/>
+      <c r="C3" s="76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="44">
+        <v>3</v>
+      </c>
+      <c r="B4" s="58"/>
+      <c r="C4" s="76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="44">
+        <v>4</v>
+      </c>
+      <c r="B5" s="58"/>
+      <c r="C5" s="76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="45">
+        <v>5</v>
+      </c>
+      <c r="B6" s="59"/>
+      <c r="C6" s="77" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="39">
+        <v>6</v>
+      </c>
+      <c r="B7" s="60" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" s="75" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="40">
+        <v>7</v>
+      </c>
+      <c r="B8" s="61"/>
+      <c r="C8" s="76">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="40">
+        <v>8</v>
+      </c>
+      <c r="B9" s="61"/>
+      <c r="C9" s="76">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="41">
+        <v>9</v>
+      </c>
+      <c r="B10" s="61"/>
+      <c r="C10" s="76">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="38">
+        <v>10</v>
+      </c>
+      <c r="B11" s="62"/>
+      <c r="C11" s="77" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="43">
+        <v>11</v>
+      </c>
+      <c r="B12" s="63" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12" s="75" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="44">
+        <v>12</v>
+      </c>
+      <c r="B13" s="64"/>
+      <c r="C13" s="76">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="44">
+        <v>13</v>
+      </c>
+      <c r="B14" s="64"/>
+      <c r="C14" s="76">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="44">
+        <v>14</v>
+      </c>
+      <c r="B15" s="64"/>
+      <c r="C15" s="76">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="45">
+        <v>15</v>
+      </c>
+      <c r="B16" s="65"/>
+      <c r="C16" s="77" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="39">
+        <v>16</v>
+      </c>
+      <c r="B17" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="C17" s="75" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="40">
+        <v>17</v>
+      </c>
+      <c r="B18" s="67"/>
+      <c r="C18" s="76">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="41">
+        <v>18</v>
+      </c>
+      <c r="B19" s="67"/>
+      <c r="C19" s="76">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="37">
+        <v>19</v>
+      </c>
+      <c r="B20" s="67"/>
+      <c r="C20" s="76">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="42">
+        <v>20</v>
+      </c>
+      <c r="B21" s="68"/>
+      <c r="C21" s="77" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="43">
+        <v>21</v>
+      </c>
+      <c r="B22" s="51" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="44">
+        <v>22</v>
+      </c>
+      <c r="B23" s="52"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="44">
+        <v>23</v>
+      </c>
+      <c r="B24" s="52"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="44">
+        <v>24</v>
+      </c>
+      <c r="B25" s="52"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="44">
+        <v>25</v>
+      </c>
+      <c r="B26" s="52"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="44">
+        <v>26</v>
+      </c>
+      <c r="B27" s="52"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="44">
+        <v>27</v>
+      </c>
+      <c r="B28" s="52"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="44">
+        <v>28</v>
+      </c>
+      <c r="B29" s="52"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="44">
+        <v>29</v>
+      </c>
+      <c r="B30" s="52"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="44">
+        <v>30</v>
+      </c>
+      <c r="B31" s="52"/>
+    </row>
+    <row r="32" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="45">
+        <v>31</v>
+      </c>
+      <c r="B32" s="53"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="36">
+        <v>32</v>
+      </c>
+      <c r="B33" s="54" t="s">
+        <v>94</v>
+      </c>
+      <c r="D33" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="37">
+        <v>33</v>
+      </c>
+      <c r="B34" s="55"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="37">
+        <v>34</v>
+      </c>
+      <c r="B35" s="55"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="37">
+        <v>35</v>
+      </c>
+      <c r="B36" s="55"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="37">
+        <v>36</v>
+      </c>
+      <c r="B37" s="55"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="37">
+        <v>37</v>
+      </c>
+      <c r="B38" s="55"/>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="37">
+        <v>38</v>
+      </c>
+      <c r="B39" s="55"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="37">
+        <v>39</v>
+      </c>
+      <c r="B40" s="55"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="37">
+        <v>40</v>
+      </c>
+      <c r="B41" s="55"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="37">
+        <v>41</v>
+      </c>
+      <c r="B42" s="55"/>
+    </row>
+    <row r="43" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="38">
+        <v>42</v>
+      </c>
+      <c r="B43" s="56"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="43">
+        <v>43</v>
+      </c>
+      <c r="B44" s="51" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="44">
+        <v>44</v>
+      </c>
+      <c r="B45" s="52"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="44">
+        <v>45</v>
+      </c>
+      <c r="B46" s="52"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="44">
+        <v>46</v>
+      </c>
+      <c r="B47" s="52"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="44">
+        <v>47</v>
+      </c>
+      <c r="B48" s="52"/>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="44">
+        <v>48</v>
+      </c>
+      <c r="B49" s="52"/>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="44">
+        <v>49</v>
+      </c>
+      <c r="B50" s="52"/>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="44">
+        <v>50</v>
+      </c>
+      <c r="B51" s="52"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="44">
+        <v>51</v>
+      </c>
+      <c r="B52" s="52"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="44">
+        <v>52</v>
+      </c>
+      <c r="B53" s="52"/>
+    </row>
+    <row r="54" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="45">
+        <v>53</v>
+      </c>
+      <c r="B54" s="53"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="36">
+        <v>54</v>
+      </c>
+      <c r="B55" s="54" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="37">
+        <v>55</v>
+      </c>
+      <c r="B56" s="55"/>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="37">
+        <v>56</v>
+      </c>
+      <c r="B57" s="55"/>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="37">
+        <v>57</v>
+      </c>
+      <c r="B58" s="55"/>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="37">
+        <v>58</v>
+      </c>
+      <c r="B59" s="55"/>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="37">
+        <v>59</v>
+      </c>
+      <c r="B60" s="55"/>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="37">
+        <v>60</v>
+      </c>
+      <c r="B61" s="55"/>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="37">
+        <v>61</v>
+      </c>
+      <c r="B62" s="55"/>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="37">
+        <v>62</v>
+      </c>
+      <c r="B63" s="55"/>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="37">
+        <v>63</v>
+      </c>
+      <c r="B64" s="55"/>
+    </row>
+    <row r="65" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="38">
+        <v>64</v>
+      </c>
+      <c r="B65" s="56"/>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="43">
+        <v>65</v>
+      </c>
+      <c r="B66" s="51" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="44">
+        <v>66</v>
+      </c>
+      <c r="B67" s="52"/>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="44">
+        <v>67</v>
+      </c>
+      <c r="B68" s="52"/>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="44">
+        <v>68</v>
+      </c>
+      <c r="B69" s="52"/>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="44">
+        <v>69</v>
+      </c>
+      <c r="B70" s="52"/>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="44">
+        <v>70</v>
+      </c>
+      <c r="B71" s="52"/>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="44">
+        <v>71</v>
+      </c>
+      <c r="B72" s="52"/>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="44">
+        <v>72</v>
+      </c>
+      <c r="B73" s="52"/>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="44">
+        <v>73</v>
+      </c>
+      <c r="B74" s="52"/>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="44">
+        <v>74</v>
+      </c>
+      <c r="B75" s="52"/>
+    </row>
+    <row r="76" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="45">
+        <v>75</v>
+      </c>
+      <c r="B76" s="53"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="B44:B54"/>
+    <mergeCell ref="B55:B65"/>
+    <mergeCell ref="B66:B76"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="B7:B11"/>
+    <mergeCell ref="B12:B16"/>
+    <mergeCell ref="B17:B21"/>
+    <mergeCell ref="B22:B32"/>
+    <mergeCell ref="B33:B43"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:Q7"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.85546875" style="15" customWidth="1"/>
+    <col min="2" max="17" width="4.140625" style="15" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="15"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="21">
+      <c r="B2" s="16">
         <v>80</v>
       </c>
-      <c r="C2" s="18">
+      <c r="C2" s="13">
         <v>81</v>
       </c>
-      <c r="D2" s="18">
+      <c r="D2" s="13">
         <v>82</v>
       </c>
-      <c r="E2" s="18">
+      <c r="E2" s="13">
         <v>83</v>
       </c>
-      <c r="F2" s="18">
+      <c r="F2" s="13">
         <v>84</v>
       </c>
-      <c r="G2" s="19">
+      <c r="G2" s="14">
         <v>85</v>
       </c>
-      <c r="H2" s="19">
+      <c r="H2" s="14">
         <v>86</v>
       </c>
-      <c r="I2" s="19">
+      <c r="I2" s="14">
         <v>87</v>
       </c>
-      <c r="J2" s="19">
+      <c r="J2" s="14">
         <v>88</v>
       </c>
-      <c r="K2" s="19">
+      <c r="K2" s="14">
         <v>89</v>
       </c>
-      <c r="L2" s="19" t="s">
+      <c r="L2" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="M2" s="19" t="s">
+      <c r="M2" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="N2" s="19" t="s">
+      <c r="N2" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="O2" s="19" t="s">
+      <c r="O2" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="P2" s="19" t="s">
+      <c r="P2" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="Q2" s="19" t="s">
+      <c r="Q2" s="14" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="3" spans="2:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="18" t="s">
+      <c r="B3" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="H3" s="23" t="s">
+      <c r="H3" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="23" t="s">
+      <c r="I3" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="J3" s="23" t="s">
+      <c r="J3" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="K3" s="23" t="s">
+      <c r="K3" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="L3" s="18" t="s">
+      <c r="L3" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="M3" s="22" t="s">
+      <c r="M3" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="N3" s="22" t="s">
+      <c r="N3" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="O3" s="22" t="s">
+      <c r="O3" s="17" t="s">
         <v>49</v>
       </c>
-      <c r="P3" s="22" t="s">
+      <c r="P3" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="Q3" s="22" t="s">
+      <c r="Q3" s="17" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="6" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="21" t="s">
+      <c r="B6" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="13"/>
+      <c r="D6" s="13"/>
+      <c r="E6" s="13"/>
+      <c r="F6" s="13"/>
+      <c r="G6" s="69" t="s">
+        <v>60</v>
+      </c>
+      <c r="H6" s="70"/>
+      <c r="I6" s="70"/>
+      <c r="J6" s="70"/>
+      <c r="K6" s="70"/>
+      <c r="L6" s="70"/>
+      <c r="M6" s="70"/>
+      <c r="N6" s="70"/>
+      <c r="O6" s="70"/>
+      <c r="P6" s="70"/>
+      <c r="Q6" s="71"/>
+    </row>
+    <row r="7" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="13"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
+      <c r="H7" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="I7" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="J7" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="K7" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="L7" s="13"/>
+      <c r="M7" s="72" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="H6" s="29"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="29"/>
-      <c r="K6" s="29"/>
-      <c r="L6" s="29"/>
-      <c r="M6" s="29"/>
-      <c r="N6" s="29"/>
-      <c r="O6" s="29"/>
-      <c r="P6" s="29"/>
-      <c r="Q6" s="30"/>
-    </row>
-    <row r="7" spans="2:17" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="23" t="s">
-        <v>57</v>
-      </c>
-      <c r="I7" s="23" t="s">
-        <v>58</v>
-      </c>
-      <c r="J7" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="K7" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="L7" s="18"/>
-      <c r="M7" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="N7" s="32"/>
-      <c r="O7" s="32"/>
-      <c r="P7" s="32"/>
-      <c r="Q7" s="33"/>
-    </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="C10" s="20" t="s">
-        <v>54</v>
-      </c>
+      <c r="N7" s="73"/>
+      <c r="O7" s="73"/>
+      <c r="P7" s="73"/>
+      <c r="Q7" s="74"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>